<commit_message>
Add problem statement and SQL script for merging products per customer by day
</commit_message>
<xml_diff>
--- a/Merge_Products/Problem_Statement.xlsx
+++ b/Merge_Products/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q9/Video_Q9_Scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Merge_Products\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5FB786-F000-3742-AD9A-E18923F20247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346D9C30-9558-484B-B2BB-66374FD098C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{67788DE1-2A4F-384B-B90C-C7BD7F35B3F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{67788DE1-2A4F-384B-B90C-C7BD7F35B3F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -51,29 +49,6 @@
   </si>
   <si>
     <t>DATES</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Video #9</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - Merge products</t>
-    </r>
   </si>
   <si>
     <t>PRODUCTS</t>
@@ -99,6 +74,29 @@
       </rPr>
       <t xml:space="preserve">
 Write an sql query to merge products per customer for each day as shown in expected output.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Merge products</t>
     </r>
   </si>
 </sst>
@@ -190,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -400,6 +398,32 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -436,7 +460,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -445,7 +468,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -465,6 +487,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -800,256 +828,208 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1279FC28-E52D-3B4A-893D-58E9E7446CC9}">
-  <dimension ref="B1:H19"/>
+  <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="4" width="15.83203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="8" width="15.83203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.796875" style="1"/>
+    <col min="2" max="4" width="15.796875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.796875" style="1"/>
+    <col min="7" max="8" width="15.796875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="20" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="2:8" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="B1" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="G6" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="27"/>
+    </row>
+    <row r="7" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-    </row>
-    <row r="2" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-    </row>
-    <row r="3" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-    </row>
-    <row r="4" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-    </row>
-    <row r="6" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8">
+        <v>45340</v>
+      </c>
+      <c r="D8" s="9">
+        <v>101</v>
+      </c>
+      <c r="G8" s="13">
+        <v>45340</v>
+      </c>
+      <c r="H8" s="14">
+        <v>101102</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="10">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11">
+        <v>45340</v>
+      </c>
+      <c r="D9" s="12">
+        <v>102</v>
+      </c>
+      <c r="G9" s="13">
+        <v>45340</v>
+      </c>
+      <c r="H9" s="14">
+        <v>104105</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11">
+        <v>45341</v>
+      </c>
+      <c r="D10" s="12">
+        <v>101</v>
+      </c>
+      <c r="G10" s="13">
+        <v>45341</v>
+      </c>
+      <c r="H10" s="14">
+        <v>101103</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+      <c r="C11" s="11">
+        <v>45341</v>
+      </c>
+      <c r="D11" s="12">
+        <v>103</v>
+      </c>
+      <c r="G11" s="13">
+        <v>45341</v>
+      </c>
+      <c r="H11" s="14">
+        <v>101106</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-      <c r="G7" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="24"/>
-    </row>
-    <row r="8" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="C12" s="11">
         <v>45340</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D12" s="12">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="10">
+        <v>2</v>
+      </c>
+      <c r="C13" s="11">
+        <v>45340</v>
+      </c>
+      <c r="D13" s="12">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="10">
+        <v>2</v>
+      </c>
+      <c r="C14" s="11">
+        <v>45341</v>
+      </c>
+      <c r="D14" s="12">
         <v>101</v>
       </c>
-      <c r="G9" s="10">
-        <v>45340</v>
-      </c>
-      <c r="H9" s="9">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="11">
-        <v>1</v>
-      </c>
-      <c r="C10" s="12">
-        <v>45340</v>
-      </c>
-      <c r="D10" s="13">
-        <v>102</v>
-      </c>
-      <c r="G10" s="14">
-        <v>45340</v>
-      </c>
-      <c r="H10" s="15">
-        <v>101102</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="12">
+    </row>
+    <row r="15" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="16">
         <v>45341</v>
       </c>
-      <c r="D11" s="13">
-        <v>101</v>
-      </c>
-      <c r="G11" s="14">
-        <v>45340</v>
-      </c>
-      <c r="H11" s="13">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="11">
-        <v>1</v>
-      </c>
-      <c r="C12" s="12">
-        <v>45341</v>
-      </c>
-      <c r="D12" s="13">
-        <v>103</v>
-      </c>
-      <c r="G12" s="14">
-        <v>45340</v>
-      </c>
-      <c r="H12" s="13">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="11">
-        <v>2</v>
-      </c>
-      <c r="C13" s="12">
-        <v>45340</v>
-      </c>
-      <c r="D13" s="13">
-        <v>104</v>
-      </c>
-      <c r="G13" s="14">
-        <v>45340</v>
-      </c>
-      <c r="H13" s="15">
-        <v>104105</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="11">
-        <v>2</v>
-      </c>
-      <c r="C14" s="12">
-        <v>45340</v>
-      </c>
-      <c r="D14" s="13">
-        <v>105</v>
-      </c>
-      <c r="G14" s="14">
-        <v>45340</v>
-      </c>
-      <c r="H14" s="13">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="11">
-        <v>2</v>
-      </c>
-      <c r="C15" s="12">
-        <v>45341</v>
-      </c>
-      <c r="D15" s="13">
-        <v>101</v>
-      </c>
-      <c r="G15" s="14">
-        <v>45341</v>
-      </c>
-      <c r="H15" s="13">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16">
-        <v>2</v>
-      </c>
-      <c r="C16" s="17">
-        <v>45341</v>
-      </c>
-      <c r="D16" s="18">
-        <v>106</v>
-      </c>
-      <c r="G16" s="14">
-        <v>45341</v>
-      </c>
-      <c r="H16" s="15">
-        <v>101103</v>
-      </c>
-    </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G17" s="14">
-        <v>45341</v>
-      </c>
-      <c r="H17" s="15">
-        <v>101106</v>
-      </c>
-    </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G18" s="14">
-        <v>45341</v>
-      </c>
-      <c r="H18" s="13">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="7:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G19" s="19">
-        <v>45341</v>
-      </c>
-      <c r="H19" s="18">
+      <c r="D15" s="17">
         <v>106</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>